<commit_message>
added schedule details to the excel file.
</commit_message>
<xml_diff>
--- a/Ayub/My Schedule.xlsx
+++ b/Ayub/My Schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="1128" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>S.No</t>
   </si>
@@ -29,6 +29,18 @@
   </si>
   <si>
     <t>Exercise Examples</t>
+  </si>
+  <si>
+    <t>Concepts of Class &amp; Object</t>
+  </si>
+  <si>
+    <t>7th June 2016</t>
+  </si>
+  <si>
+    <t>14th June 2016</t>
+  </si>
+  <si>
+    <t>console application with class &amp; object</t>
   </si>
 </sst>
 </file>
@@ -93,11 +105,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,16 +418,16 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -437,6 +450,18 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Schedule excel sheet
</commit_message>
<xml_diff>
--- a/Ayub/My Schedule.xlsx
+++ b/Ayub/My Schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1128" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="2016" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>S.No</t>
   </si>
@@ -41,6 +41,15 @@
   </si>
   <si>
     <t>console application with class &amp; object</t>
+  </si>
+  <si>
+    <t>Data Types, Variables, Properties &amp; methods. Arithmetic operations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14th June 2016 </t>
+  </si>
+  <si>
+    <t>21st june 2016</t>
   </si>
 </sst>
 </file>
@@ -105,12 +114,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,16 +429,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.21875" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
     <col min="5" max="5" width="40.5546875" customWidth="1"/>
@@ -448,21 +462,78 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>